<commit_message>
fix: updated the excel import feature for category field.
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Beispiel.xlsx
+++ b/src/main/resources/templates/excel/Beispiel.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gst\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV555\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B10894-DB69-45B4-BA40-E17C962064DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD29EF37-6986-4350-9AA5-51613CBCF68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27660" yWindow="6255" windowWidth="22605" windowHeight="14670" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
   </bookViews>
   <sheets>
     <sheet name="DubbleBeispiel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Kundennummer</t>
   </si>
@@ -91,6 +82,36 @@
   </si>
   <si>
     <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Sus</t>
+  </si>
+  <si>
+    <t>Tefy</t>
+  </si>
+  <si>
+    <t>F GB h</t>
+  </si>
+  <si>
+    <t>Gdgh</t>
+  </si>
+  <si>
+    <t>Ghdc@gcfdb.fh</t>
+  </si>
+  <si>
+    <t>Ggsd@jhvt.yfg</t>
+  </si>
+  <si>
+    <t>Apple|Microsoft</t>
+  </si>
+  <si>
+    <t>Dell|Apple</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Dell|Microsoft Azure</t>
   </si>
 </sst>
 </file>
@@ -135,17 +156,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -161,7 +183,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -457,13 +479,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6436DEE0-B104-4F83-B38D-6A60E7FE1769}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
@@ -522,6 +544,9 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -541,12 +566,45 @@
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{94C89386-6AB0-4F55-BCB6-8B42687B64A5}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{7ADB0177-025D-4BA2-BF1C-501B390079F9}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{9ED13072-6BCC-3140-86CC-1647692F6DBC}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{EFC96D1F-5337-9846-9FE3-E4CAD9BDC606}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: implemented the company feature for customer
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Beispiel.xlsx
+++ b/src/main/resources/templates/excel/Beispiel.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV555\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gst\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD29EF37-6986-4350-9AA5-51613CBCF68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89109E5B-00AC-499A-B857-AB7C032C81F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
+    <workbookView xWindow="-21045" yWindow="5730" windowWidth="16545" windowHeight="15525" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
   </bookViews>
   <sheets>
     <sheet name="DubbleBeispiel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Kundennummer</t>
   </si>
@@ -66,52 +75,13 @@
     <t>+4300000000</t>
   </si>
   <si>
-    <t>A4567</t>
-  </si>
-  <si>
-    <t>Maxime</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>maxi.mustermann@aon.at</t>
-  </si>
-  <si>
-    <t>+435000000</t>
-  </si>
-  <si>
     <t>Kategorie</t>
   </si>
   <si>
-    <t>Sus</t>
-  </si>
-  <si>
-    <t>Tefy</t>
-  </si>
-  <si>
-    <t>F GB h</t>
-  </si>
-  <si>
-    <t>Gdgh</t>
-  </si>
-  <si>
-    <t>Ghdc@gcfdb.fh</t>
-  </si>
-  <si>
-    <t>Ggsd@jhvt.yfg</t>
-  </si>
-  <si>
-    <t>Apple|Microsoft</t>
-  </si>
-  <si>
-    <t>Dell|Apple</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>Dell|Microsoft Azure</t>
+    <t>Unternehmen</t>
+  </si>
+  <si>
+    <t>Max Mustermann GmbH</t>
   </si>
 </sst>
 </file>
@@ -167,7 +137,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -183,7 +153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -479,13 +449,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6436DEE0-B104-4F83-B38D-6A60E7FE1769}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
@@ -494,9 +464,10 @@
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,11 +489,14 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>123456</v>
       </c>
@@ -544,67 +518,22 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{94C89386-6AB0-4F55-BCB6-8B42687B64A5}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{7ADB0177-025D-4BA2-BF1C-501B390079F9}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{9ED13072-6BCC-3140-86CC-1647692F6DBC}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{EFC96D1F-5337-9846-9FE3-E4CAD9BDC606}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: modified the cell name of excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Beispiel.xlsx
+++ b/src/main/resources/templates/excel/Beispiel.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gst\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Workspace\Web\freelance-project\dubble_backend\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89109E5B-00AC-499A-B857-AB7C032C81F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D57267-7863-4996-8EEF-D98F44541C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21045" yWindow="5730" windowWidth="16545" windowHeight="15525" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
   </bookViews>
   <sheets>
     <sheet name="DubbleBeispiel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -75,13 +66,13 @@
     <t>+4300000000</t>
   </si>
   <si>
-    <t>Kategorie</t>
-  </si>
-  <si>
     <t>Unternehmen</t>
   </si>
   <si>
     <t>Max Mustermann GmbH</t>
+  </si>
+  <si>
+    <t>Kunden Interessen</t>
   </si>
 </sst>
 </file>
@@ -137,7 +128,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -153,7 +144,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,10 +443,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
@@ -465,6 +456,7 @@
     <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -490,10 +482,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -519,7 +511,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: modified the title of excel data
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Beispiel.xlsx
+++ b/src/main/resources/templates/excel/Beispiel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Workspace\Web\freelance-project\dubble_backend\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73389879-D7A7-4042-9826-8A23A7F1C206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A342EA22-D858-4ADD-8697-B0F7BD395062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DDD63B73-0346-4644-8C53-61C190B4C8B1}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>eMail</t>
   </si>
   <si>
-    <t>Telefonnummer(+43…)</t>
-  </si>
-  <si>
     <t>Dr</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Kunden_Interessen</t>
+  </si>
+  <si>
+    <t>Mobilnummer(+43…)</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,13 +479,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -493,25 +493,25 @@
         <v>123456</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>